<commit_message>
chore(data): add 2026-1 data files ('26.01.15)
</commit_message>
<xml_diff>
--- a/data/2026년 1학기 정규 시간표.xlsx
+++ b/data/2026년 1학기 정규 시간표.xlsx
@@ -688,7 +688,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>금2</t>
+          <t>수2</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -14833,7 +14833,7 @@
       </c>
       <c r="K239" t="inlineStr">
         <is>
-          <t>제2과학관106호강의실</t>
+          <t>요한관421호(中)강의실</t>
         </is>
       </c>
       <c r="L239" t="inlineStr">
@@ -19365,7 +19365,11 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I313" t="inlineStr"/>
+      <c r="I313" t="inlineStr">
+        <is>
+          <t>강민승</t>
+        </is>
+      </c>
       <c r="J313" t="inlineStr">
         <is>
           <t>화5~6</t>
@@ -19685,7 +19689,11 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I318" t="inlineStr"/>
+      <c r="I318" t="inlineStr">
+        <is>
+          <t>허상민</t>
+        </is>
+      </c>
       <c r="J318" t="inlineStr">
         <is>
           <t>화5~6</t>
@@ -19757,7 +19765,7 @@
       </c>
       <c r="K319" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>요한관 홍명기홀(강당)</t>
         </is>
       </c>
       <c r="L319" t="inlineStr">
@@ -24905,7 +24913,7 @@
       </c>
       <c r="K405" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>대강당(메인)</t>
         </is>
       </c>
       <c r="L405" t="inlineStr">
@@ -24969,7 +24977,7 @@
       </c>
       <c r="K406" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>대강당(메인)</t>
         </is>
       </c>
       <c r="L406" t="inlineStr">
@@ -25821,7 +25829,7 @@
       </c>
       <c r="K421" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>에스라관114호(大)강의실,제2과학관106호강의실</t>
         </is>
       </c>
       <c r="L421" t="inlineStr">
@@ -25881,7 +25889,7 @@
       </c>
       <c r="K422" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>바울관203호(PBL)강의실</t>
         </is>
       </c>
       <c r="L422" t="inlineStr">
@@ -26225,7 +26233,7 @@
       </c>
       <c r="K428" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>사무엘관208호강의실</t>
         </is>
       </c>
       <c r="L428" t="inlineStr">
@@ -26285,7 +26293,7 @@
       </c>
       <c r="K429" t="inlineStr">
         <is>
-          <t>미지정,바울관306호강의실</t>
+          <t>다니엘관302호(中)강의실,바울관306호강의실</t>
         </is>
       </c>
       <c r="L429" t="inlineStr">
@@ -26345,7 +26353,7 @@
       </c>
       <c r="K430" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>다니엘관208호(大)강의실,제2과학관106호강의실</t>
         </is>
       </c>
       <c r="L430" t="inlineStr">
@@ -26461,7 +26469,7 @@
       </c>
       <c r="K432" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>신학관210호강의실</t>
         </is>
       </c>
       <c r="L432" t="inlineStr">
@@ -26753,7 +26761,7 @@
       </c>
       <c r="K437" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>다니엘관202호(小)강의실</t>
         </is>
       </c>
       <c r="L437" t="inlineStr">
@@ -26813,7 +26821,7 @@
       </c>
       <c r="K438" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>다니엘관201호(小)강의실</t>
         </is>
       </c>
       <c r="L438" t="inlineStr">
@@ -28058,16 +28066,8 @@
           <t>Lee Jeeny Jeeyoun</t>
         </is>
       </c>
-      <c r="J459" t="inlineStr">
-        <is>
-          <t>화5~7</t>
-        </is>
-      </c>
-      <c r="K459" t="inlineStr">
-        <is>
-          <t>체육관309호(中)강의실</t>
-        </is>
-      </c>
+      <c r="J459" t="inlineStr"/>
+      <c r="K459" t="inlineStr"/>
       <c r="L459" t="inlineStr">
         <is>
           <t>미래융합대학</t>
@@ -28289,7 +28289,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I463" t="inlineStr"/>
+      <c r="I463" t="inlineStr">
+        <is>
+          <t>홍지훈</t>
+        </is>
+      </c>
       <c r="J463" t="inlineStr">
         <is>
           <t>수5~7</t>
@@ -29177,7 +29181,7 @@
       </c>
       <c r="K478" t="inlineStr">
         <is>
-          <t>사무엘관209호강의실</t>
+          <t>국제교육관221호(中)강의실</t>
         </is>
       </c>
       <c r="L478" t="inlineStr">
@@ -29866,8 +29870,16 @@
         </is>
       </c>
       <c r="I490" t="inlineStr"/>
-      <c r="J490" t="inlineStr"/>
-      <c r="K490" t="inlineStr"/>
+      <c r="J490" t="inlineStr">
+        <is>
+          <t>금1~4</t>
+        </is>
+      </c>
+      <c r="K490" t="inlineStr">
+        <is>
+          <t>제1실습관202호강의실</t>
+        </is>
+      </c>
       <c r="L490" t="inlineStr">
         <is>
           <t>미래융합대학</t>
@@ -30394,8 +30406,16 @@
         </is>
       </c>
       <c r="I499" t="inlineStr"/>
-      <c r="J499" t="inlineStr"/>
-      <c r="K499" t="inlineStr"/>
+      <c r="J499" t="inlineStr">
+        <is>
+          <t>금5~7</t>
+        </is>
+      </c>
+      <c r="K499" t="inlineStr">
+        <is>
+          <t>제1실습관202호강의실</t>
+        </is>
+      </c>
       <c r="L499" t="inlineStr">
         <is>
           <t>미래융합대학</t>
@@ -31314,8 +31334,16 @@
         </is>
       </c>
       <c r="I515" t="inlineStr"/>
-      <c r="J515" t="inlineStr"/>
-      <c r="K515" t="inlineStr"/>
+      <c r="J515" t="inlineStr">
+        <is>
+          <t>금2~4</t>
+        </is>
+      </c>
+      <c r="K515" t="inlineStr">
+        <is>
+          <t>요한관423호(中)강의실</t>
+        </is>
+      </c>
       <c r="L515" t="inlineStr">
         <is>
           <t>미래융합대학</t>
@@ -31593,7 +31621,11 @@
           <t>0</t>
         </is>
       </c>
-      <c r="I520" t="inlineStr"/>
+      <c r="I520" t="inlineStr">
+        <is>
+          <t>이한청</t>
+        </is>
+      </c>
       <c r="J520" t="inlineStr">
         <is>
           <t>화1~3</t>
@@ -31653,7 +31685,11 @@
           <t>0</t>
         </is>
       </c>
-      <c r="I521" t="inlineStr"/>
+      <c r="I521" t="inlineStr">
+        <is>
+          <t>이한청</t>
+        </is>
+      </c>
       <c r="J521" t="inlineStr">
         <is>
           <t>목4~6</t>
@@ -31713,7 +31749,11 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I522" t="inlineStr"/>
+      <c r="I522" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="J522" t="inlineStr">
         <is>
           <t>월5~6</t>
@@ -32917,7 +32957,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I541" t="inlineStr"/>
+      <c r="I541" t="inlineStr">
+        <is>
+          <t>정수목</t>
+        </is>
+      </c>
       <c r="J541" t="inlineStr">
         <is>
           <t>목2~4</t>
@@ -32977,7 +33021,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I542" t="inlineStr"/>
+      <c r="I542" t="inlineStr">
+        <is>
+          <t>정수목</t>
+        </is>
+      </c>
       <c r="J542" t="inlineStr">
         <is>
           <t>금2~4</t>
@@ -33293,7 +33341,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I548" t="inlineStr"/>
+      <c r="I548" t="inlineStr">
+        <is>
+          <t>조충희</t>
+        </is>
+      </c>
       <c r="J548" t="inlineStr">
         <is>
           <t>월1~3</t>
@@ -33353,7 +33405,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I549" t="inlineStr"/>
+      <c r="I549" t="inlineStr">
+        <is>
+          <t>조충희</t>
+        </is>
+      </c>
       <c r="J549" t="inlineStr">
         <is>
           <t>월5~7</t>
@@ -34630,16 +34686,8 @@
           <t>미지정</t>
         </is>
       </c>
-      <c r="J570" t="inlineStr">
-        <is>
-          <t>화1~3</t>
-        </is>
-      </c>
-      <c r="K570" t="inlineStr">
-        <is>
-          <t>미지정</t>
-        </is>
-      </c>
+      <c r="J570" t="inlineStr"/>
+      <c r="K570" t="inlineStr"/>
       <c r="L570" t="inlineStr">
         <is>
           <t>미래융합대학</t>
@@ -34647,7 +34695,7 @@
       </c>
       <c r="M570" t="inlineStr">
         <is>
-          <t>홀수학번(A반)</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N570" t="inlineStr"/>
@@ -34694,16 +34742,8 @@
           <t>미지정</t>
         </is>
       </c>
-      <c r="J571" t="inlineStr">
-        <is>
-          <t>화4~6</t>
-        </is>
-      </c>
-      <c r="K571" t="inlineStr">
-        <is>
-          <t>미지정</t>
-        </is>
-      </c>
+      <c r="J571" t="inlineStr"/>
+      <c r="K571" t="inlineStr"/>
       <c r="L571" t="inlineStr">
         <is>
           <t>미래융합대학</t>
@@ -34711,7 +34751,7 @@
       </c>
       <c r="M571" t="inlineStr">
         <is>
-          <t>짝수학번(B반)</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N571" t="inlineStr"/>
@@ -38885,11 +38925,7 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I641" t="inlineStr">
-        <is>
-          <t>미지정</t>
-        </is>
-      </c>
+      <c r="I641" t="inlineStr"/>
       <c r="J641" t="inlineStr">
         <is>
           <t>목2~3</t>
@@ -38897,7 +38933,7 @@
       </c>
       <c r="K641" t="inlineStr">
         <is>
-          <t>제2과학관501-1호강의실</t>
+          <t>다니엘관305호(大)</t>
         </is>
       </c>
       <c r="L641" t="inlineStr">
@@ -39191,7 +39227,7 @@
       </c>
       <c r="I646" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>김은아</t>
         </is>
       </c>
       <c r="J646" t="inlineStr">
@@ -39875,7 +39911,7 @@
       </c>
       <c r="I657" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>유재형</t>
         </is>
       </c>
       <c r="J657" t="inlineStr">
@@ -40607,7 +40643,7 @@
       </c>
       <c r="I669" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>유재형</t>
         </is>
       </c>
       <c r="J669" t="inlineStr">
@@ -40965,11 +41001,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I675" t="inlineStr">
-        <is>
-          <t>미지정</t>
-        </is>
-      </c>
+      <c r="I675" t="inlineStr"/>
       <c r="J675" t="inlineStr">
         <is>
           <t>화1~3</t>
@@ -41807,7 +41839,7 @@
       </c>
       <c r="I689" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>이창래</t>
         </is>
       </c>
       <c r="J689" t="inlineStr">
@@ -41867,7 +41899,7 @@
       </c>
       <c r="I690" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>한행하</t>
         </is>
       </c>
       <c r="J690" t="inlineStr">
@@ -51037,7 +51069,7 @@
       </c>
       <c r="K842" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>바울관214호강의실</t>
         </is>
       </c>
       <c r="L842" t="inlineStr">
@@ -53045,7 +53077,7 @@
       </c>
       <c r="K874" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>바울관213호강의실(대학원전용)</t>
         </is>
       </c>
       <c r="L874" t="inlineStr">
@@ -55870,8 +55902,16 @@
           <t>취업정보</t>
         </is>
       </c>
-      <c r="J921" t="inlineStr"/>
-      <c r="K921" t="inlineStr"/>
+      <c r="J921" t="inlineStr">
+        <is>
+          <t>화7~8</t>
+        </is>
+      </c>
+      <c r="K921" t="inlineStr">
+        <is>
+          <t>에스라관406호강의실(첨단강의실)</t>
+        </is>
+      </c>
       <c r="L921" t="inlineStr">
         <is>
           <t>창의융합대학</t>
@@ -55930,8 +55970,16 @@
           <t>취업정보</t>
         </is>
       </c>
-      <c r="J922" t="inlineStr"/>
-      <c r="K922" t="inlineStr"/>
+      <c r="J922" t="inlineStr">
+        <is>
+          <t>목5~6</t>
+        </is>
+      </c>
+      <c r="K922" t="inlineStr">
+        <is>
+          <t>다니엘관402호(PBL)강의실</t>
+        </is>
+      </c>
       <c r="L922" t="inlineStr">
         <is>
           <t>창의융합대학</t>
@@ -55990,8 +56038,16 @@
           <t>취업정보</t>
         </is>
       </c>
-      <c r="J923" t="inlineStr"/>
-      <c r="K923" t="inlineStr"/>
+      <c r="J923" t="inlineStr">
+        <is>
+          <t>화5~6</t>
+        </is>
+      </c>
+      <c r="K923" t="inlineStr">
+        <is>
+          <t>백주년311호강의실</t>
+        </is>
+      </c>
       <c r="L923" t="inlineStr">
         <is>
           <t>창의융합대학</t>
@@ -56958,8 +57014,16 @@
           <t>이규일</t>
         </is>
       </c>
-      <c r="J938" t="inlineStr"/>
-      <c r="K938" t="inlineStr"/>
+      <c r="J938" t="inlineStr">
+        <is>
+          <t>화1~2</t>
+        </is>
+      </c>
+      <c r="K938" t="inlineStr">
+        <is>
+          <t>사무엘관210호(PBL소형)강의실</t>
+        </is>
+      </c>
       <c r="L938" t="inlineStr">
         <is>
           <t>창의융합대학</t>
@@ -57562,8 +57626,16 @@
           <t>안병삼</t>
         </is>
       </c>
-      <c r="J947" t="inlineStr"/>
-      <c r="K947" t="inlineStr"/>
+      <c r="J947" t="inlineStr">
+        <is>
+          <t>월7~8</t>
+        </is>
+      </c>
+      <c r="K947" t="inlineStr">
+        <is>
+          <t>사무엘관202호강의실</t>
+        </is>
+      </c>
       <c r="L947" t="inlineStr">
         <is>
           <t>창의융합대학</t>
@@ -58737,7 +58809,7 @@
       </c>
       <c r="K965" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>요한관421호(中)강의실</t>
         </is>
       </c>
       <c r="L965" t="inlineStr">
@@ -61257,7 +61329,7 @@
       </c>
       <c r="K1003" t="inlineStr">
         <is>
-          <t>백주년311</t>
+          <t>백주년311호강의실</t>
         </is>
       </c>
       <c r="L1003" t="inlineStr">
@@ -61325,7 +61397,7 @@
       </c>
       <c r="K1004" t="inlineStr">
         <is>
-          <t>백주년311</t>
+          <t>백주년311호강의실</t>
         </is>
       </c>
       <c r="L1004" t="inlineStr">
@@ -61393,7 +61465,7 @@
       </c>
       <c r="K1005" t="inlineStr">
         <is>
-          <t>백주년311</t>
+          <t>백주년311호강의실</t>
         </is>
       </c>
       <c r="L1005" t="inlineStr">
@@ -61461,7 +61533,7 @@
       </c>
       <c r="K1006" t="inlineStr">
         <is>
-          <t>백주년311</t>
+          <t>백주년311호강의실</t>
         </is>
       </c>
       <c r="L1006" t="inlineStr">
@@ -65233,7 +65305,7 @@
       </c>
       <c r="K1062" t="inlineStr">
         <is>
-          <t>국제교육관221호(中)강의실</t>
+          <t>사무엘관209호강의실</t>
         </is>
       </c>
       <c r="L1062" t="inlineStr">
@@ -68522,8 +68594,16 @@
           <t>홍선미</t>
         </is>
       </c>
-      <c r="J1111" t="inlineStr"/>
-      <c r="K1111" t="inlineStr"/>
+      <c r="J1111" t="inlineStr">
+        <is>
+          <t>수5~7</t>
+        </is>
+      </c>
+      <c r="K1111" t="inlineStr">
+        <is>
+          <t>사무엘관109호강의실</t>
+        </is>
+      </c>
       <c r="L1111" t="inlineStr">
         <is>
           <t>창의융합대학</t>
@@ -68997,7 +69077,7 @@
       </c>
       <c r="K1118" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>신학관208호(PBL소형)강의실</t>
         </is>
       </c>
       <c r="L1118" t="inlineStr">
@@ -69469,7 +69549,7 @@
       </c>
       <c r="K1125" t="inlineStr">
         <is>
-          <t>사무엘관110호강의실</t>
+          <t>요한관222호(中)(교필토익전용)강의실</t>
         </is>
       </c>
       <c r="L1125" t="inlineStr">
@@ -70693,7 +70773,7 @@
       </c>
       <c r="K1143" t="inlineStr">
         <is>
-          <t>요한관222호(中)(교필토익전용)강의실</t>
+          <t>사무엘관110호강의실</t>
         </is>
       </c>
       <c r="L1143" t="inlineStr">
@@ -70953,7 +71033,7 @@
       </c>
       <c r="K1147" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>사무엘관202호강의실</t>
         </is>
       </c>
       <c r="L1147" t="inlineStr">
@@ -71781,7 +71861,7 @@
       </c>
       <c r="K1160" t="inlineStr">
         <is>
-          <t>에스라관405호 한국어문화실습실</t>
+          <t>에스라관113호강의실</t>
         </is>
       </c>
       <c r="L1160" t="inlineStr">
@@ -73921,7 +74001,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1195" t="inlineStr"/>
+      <c r="I1195" t="inlineStr">
+        <is>
+          <t>박혁준</t>
+        </is>
+      </c>
       <c r="J1195" t="inlineStr">
         <is>
           <t>월2~4</t>
@@ -77051,7 +77135,7 @@
       </c>
       <c r="I1247" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>안류연</t>
         </is>
       </c>
       <c r="J1247" t="inlineStr">
@@ -77351,7 +77435,7 @@
       </c>
       <c r="I1252" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>안류연</t>
         </is>
       </c>
       <c r="J1252" t="inlineStr">
@@ -77361,7 +77445,7 @@
       </c>
       <c r="K1252" t="inlineStr">
         <is>
-          <t>바울관313호강의실</t>
+          <t>사무엘관309호(大)강의실</t>
         </is>
       </c>
       <c r="L1252" t="inlineStr">
@@ -80447,12 +80531,12 @@
       </c>
       <c r="I1303" t="inlineStr">
         <is>
-          <t>조혜령</t>
+          <t>윤진영</t>
         </is>
       </c>
       <c r="J1303" t="inlineStr">
         <is>
-          <t>목5~7</t>
+          <t>금5~7</t>
         </is>
       </c>
       <c r="K1303" t="inlineStr">
@@ -80507,12 +80591,12 @@
       </c>
       <c r="I1304" t="inlineStr">
         <is>
-          <t>조혜령</t>
+          <t>윤진영</t>
         </is>
       </c>
       <c r="J1304" t="inlineStr">
         <is>
-          <t>목1~3</t>
+          <t>금1~3</t>
         </is>
       </c>
       <c r="K1304" t="inlineStr">
@@ -82691,7 +82775,7 @@
       </c>
       <c r="I1340" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>LagundinoWilliamChester</t>
         </is>
       </c>
       <c r="J1340" t="inlineStr">
@@ -83115,7 +83199,7 @@
       </c>
       <c r="I1347" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>로즈마리신</t>
         </is>
       </c>
       <c r="J1347" t="inlineStr">
@@ -83178,8 +83262,16 @@
           <t>교목처</t>
         </is>
       </c>
-      <c r="J1348" t="inlineStr"/>
-      <c r="K1348" t="inlineStr"/>
+      <c r="J1348" t="inlineStr">
+        <is>
+          <t>금0</t>
+        </is>
+      </c>
+      <c r="K1348" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1348" t="inlineStr">
         <is>
           <t>창의융합대학</t>
@@ -83587,7 +83679,7 @@
       </c>
       <c r="I1355" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>Ian Robert J.Aujero</t>
         </is>
       </c>
       <c r="J1355" t="inlineStr">
@@ -83597,7 +83689,7 @@
       </c>
       <c r="K1355" t="inlineStr">
         <is>
-          <t>사무엘관308호(특수)강의실</t>
+          <t>사무엘관209호강의실,사무엘관308호(특수)강의실</t>
         </is>
       </c>
       <c r="L1355" t="inlineStr">
@@ -83717,7 +83809,7 @@
       </c>
       <c r="K1357" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>대강당(메인)</t>
         </is>
       </c>
       <c r="L1357" t="inlineStr">
@@ -83781,7 +83873,7 @@
       </c>
       <c r="K1358" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>대강당(메인)</t>
         </is>
       </c>
       <c r="L1358" t="inlineStr">
@@ -83895,7 +83987,7 @@
       </c>
       <c r="I1360" t="inlineStr">
         <is>
-          <t>안병구</t>
+          <t>미지정</t>
         </is>
       </c>
       <c r="J1360" t="inlineStr">
@@ -84261,7 +84353,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1366" t="inlineStr"/>
+      <c r="I1366" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="J1366" t="inlineStr">
         <is>
           <t>목1~3</t>
@@ -84629,7 +84725,7 @@
       </c>
       <c r="K1372" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제1실습관304호강의실(유교과)</t>
         </is>
       </c>
       <c r="L1372" t="inlineStr">
@@ -84885,7 +84981,7 @@
       </c>
       <c r="K1376" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제1실습관304호강의실(유교과)</t>
         </is>
       </c>
       <c r="L1376" t="inlineStr">
@@ -85129,7 +85225,7 @@
       </c>
       <c r="K1380" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제1실습관304호강의실(유교과)</t>
         </is>
       </c>
       <c r="L1380" t="inlineStr">
@@ -85193,7 +85289,7 @@
       </c>
       <c r="K1381" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제1실습관304호강의실(유교과)</t>
         </is>
       </c>
       <c r="L1381" t="inlineStr">
@@ -85257,7 +85353,7 @@
       </c>
       <c r="K1382" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제1실습관307호(토의·토론 세미나실)</t>
         </is>
       </c>
       <c r="L1382" t="inlineStr">
@@ -85377,7 +85473,7 @@
       </c>
       <c r="K1384" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제1실습관304호강의실(유교과)</t>
         </is>
       </c>
       <c r="L1384" t="inlineStr">
@@ -85437,7 +85533,7 @@
       </c>
       <c r="K1385" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>온라인(가상공간)</t>
         </is>
       </c>
       <c r="L1385" t="inlineStr">
@@ -85561,7 +85657,7 @@
       </c>
       <c r="K1387" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제1실습관307호(토의·토론 세미나실)</t>
         </is>
       </c>
       <c r="L1387" t="inlineStr">
@@ -85625,7 +85721,7 @@
       </c>
       <c r="K1388" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제1실습관307호(토의·토론 세미나실)</t>
         </is>
       </c>
       <c r="L1388" t="inlineStr">
@@ -85689,7 +85785,7 @@
       </c>
       <c r="K1389" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제1실습관307호(토의·토론 세미나실)</t>
         </is>
       </c>
       <c r="L1389" t="inlineStr">
@@ -85809,7 +85905,7 @@
       </c>
       <c r="K1391" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제1실습관304호강의실(유교과)</t>
         </is>
       </c>
       <c r="L1391" t="inlineStr">
@@ -85869,7 +85965,7 @@
       </c>
       <c r="K1392" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제1실습관304호강의실(유교과)</t>
         </is>
       </c>
       <c r="L1392" t="inlineStr">
@@ -85929,7 +86025,7 @@
       </c>
       <c r="K1393" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제1실습관304호강의실(유교과)</t>
         </is>
       </c>
       <c r="L1393" t="inlineStr">
@@ -92344,7 +92440,7 @@
       </c>
       <c r="J1497" t="inlineStr">
         <is>
-          <t>수2~3</t>
+          <t>금3~4</t>
         </is>
       </c>
       <c r="K1497" t="inlineStr">
@@ -92948,7 +93044,7 @@
       </c>
       <c r="J1507" t="inlineStr">
         <is>
-          <t>수5~6</t>
+          <t>금1~2</t>
         </is>
       </c>
       <c r="K1507" t="inlineStr">
@@ -93488,7 +93584,7 @@
       <c r="I1516" t="inlineStr"/>
       <c r="J1516" t="inlineStr">
         <is>
-          <t>목4~5</t>
+          <t>목5~6</t>
         </is>
       </c>
       <c r="K1516" t="inlineStr">
@@ -93601,7 +93697,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1518" t="inlineStr"/>
+      <c r="I1518" t="inlineStr">
+        <is>
+          <t>이준민</t>
+        </is>
+      </c>
       <c r="J1518" t="inlineStr">
         <is>
           <t>월2~4</t>
@@ -93609,7 +93709,7 @@
       </c>
       <c r="K1518" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>다니엘관406호(PBL 전용 Lab. 中)강의실</t>
         </is>
       </c>
       <c r="L1518" t="inlineStr">
@@ -93669,7 +93769,7 @@
       </c>
       <c r="K1519" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>체육관309호(中)강의실</t>
         </is>
       </c>
       <c r="L1519" t="inlineStr">
@@ -94325,7 +94425,7 @@
       </c>
       <c r="K1530" t="inlineStr">
         <is>
-          <t>체육관309호(中)강의실</t>
+          <t>체육관308호(中)강의실</t>
         </is>
       </c>
       <c r="L1530" t="inlineStr">
@@ -94385,7 +94485,7 @@
       </c>
       <c r="K1531" t="inlineStr">
         <is>
-          <t>체육관309호(中)강의실</t>
+          <t>바울관301호(컴퓨터실)</t>
         </is>
       </c>
       <c r="L1531" t="inlineStr">

</xml_diff>

<commit_message>
chore(data): add 2026-1 data files ('26.01.17)
</commit_message>
<xml_diff>
--- a/data/2026년 1학기 정규 시간표.xlsx
+++ b/data/2026년 1학기 정규 시간표.xlsx
@@ -15309,7 +15309,7 @@
       </c>
       <c r="K247" t="inlineStr">
         <is>
-          <t>제2과학관208호(동물영양사료분석실)</t>
+          <t>요한관224호(中)강의실</t>
         </is>
       </c>
       <c r="L247" t="inlineStr">
@@ -15373,7 +15373,7 @@
       </c>
       <c r="K248" t="inlineStr">
         <is>
-          <t>제2과학관106호강의실</t>
+          <t>국제교육관222호(中)강의실</t>
         </is>
       </c>
       <c r="L248" t="inlineStr">
@@ -16037,7 +16037,7 @@
       </c>
       <c r="K259" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제2과학관102호(세미나실)</t>
         </is>
       </c>
       <c r="L259" t="inlineStr">
@@ -16101,7 +16101,7 @@
       </c>
       <c r="K260" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제2과학관102호(세미나실)</t>
         </is>
       </c>
       <c r="L260" t="inlineStr">
@@ -16165,7 +16165,7 @@
       </c>
       <c r="K261" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제2과학관102호(세미나실)</t>
         </is>
       </c>
       <c r="L261" t="inlineStr">
@@ -16948,12 +16948,12 @@
       </c>
       <c r="J274" t="inlineStr">
         <is>
-          <t>목5~7</t>
+          <t>수2~4</t>
         </is>
       </c>
       <c r="K274" t="inlineStr">
         <is>
-          <t>다니엘관304호(大)</t>
+          <t>다니엘관405호(大)강의실</t>
         </is>
       </c>
       <c r="L274" t="inlineStr">
@@ -18344,12 +18344,12 @@
       </c>
       <c r="J297" t="inlineStr">
         <is>
-          <t>월10</t>
+          <t>월1,목13</t>
         </is>
       </c>
       <c r="K297" t="inlineStr">
         <is>
-          <t>다니엘관107호(자유전공학부 전용)</t>
+          <t>다니엘관107호(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L297" t="inlineStr">
@@ -18403,17 +18403,17 @@
       </c>
       <c r="I298" t="inlineStr">
         <is>
-          <t>김향일</t>
+          <t>노동욱</t>
         </is>
       </c>
       <c r="J298" t="inlineStr">
         <is>
-          <t>월10</t>
+          <t>월1,목13</t>
         </is>
       </c>
       <c r="K298" t="inlineStr">
         <is>
-          <t>다니엘관B102호(大)(자유전공학부 전용)</t>
+          <t>다니엘관B101호(大)(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L298" t="inlineStr">
@@ -18472,12 +18472,12 @@
       </c>
       <c r="J299" t="inlineStr">
         <is>
-          <t>화10</t>
+          <t>월3,목13</t>
         </is>
       </c>
       <c r="K299" t="inlineStr">
         <is>
-          <t>다니엘관B102호(大)(자유전공학부 전용)</t>
+          <t>다니엘관B102호(大)(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L299" t="inlineStr">
@@ -18536,12 +18536,12 @@
       </c>
       <c r="J300" t="inlineStr">
         <is>
-          <t>화10</t>
+          <t>월3,목13</t>
         </is>
       </c>
       <c r="K300" t="inlineStr">
         <is>
-          <t>다니엘관107호(자유전공학부 전용)</t>
+          <t>다니엘관107호(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L300" t="inlineStr">
@@ -18600,7 +18600,7 @@
       </c>
       <c r="J301" t="inlineStr">
         <is>
-          <t>수10</t>
+          <t>목13,목3</t>
         </is>
       </c>
       <c r="K301" t="inlineStr">
@@ -18664,12 +18664,12 @@
       </c>
       <c r="J302" t="inlineStr">
         <is>
-          <t>수10</t>
+          <t>목13,목3</t>
         </is>
       </c>
       <c r="K302" t="inlineStr">
         <is>
-          <t>다니엘관B101호(大)(자유전공학부 전용)</t>
+          <t>다니엘관B101호(大)(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L302" t="inlineStr">
@@ -18723,17 +18723,17 @@
       </c>
       <c r="I303" t="inlineStr">
         <is>
-          <t>노동욱</t>
+          <t>김향일</t>
         </is>
       </c>
       <c r="J303" t="inlineStr">
         <is>
-          <t>목10</t>
+          <t>목1,목13</t>
         </is>
       </c>
       <c r="K303" t="inlineStr">
         <is>
-          <t>다니엘관B101호(大)(자유전공학부 전용)</t>
+          <t>다니엘관B102호(大)(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L303" t="inlineStr">
@@ -18792,12 +18792,12 @@
       </c>
       <c r="J304" t="inlineStr">
         <is>
-          <t>목10</t>
+          <t>목1,목13</t>
         </is>
       </c>
       <c r="K304" t="inlineStr">
         <is>
-          <t>다니엘관107호(자유전공학부 전용)</t>
+          <t>다니엘관107호(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L304" t="inlineStr">
@@ -18856,12 +18856,12 @@
       </c>
       <c r="J305" t="inlineStr">
         <is>
-          <t>월11</t>
+          <t>월2,목13</t>
         </is>
       </c>
       <c r="K305" t="inlineStr">
         <is>
-          <t>다니엘관107호(자유전공학부 전용)</t>
+          <t>다니엘관107호(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L305" t="inlineStr">
@@ -18915,17 +18915,17 @@
       </c>
       <c r="I306" t="inlineStr">
         <is>
-          <t>김향일</t>
+          <t>노동욱</t>
         </is>
       </c>
       <c r="J306" t="inlineStr">
         <is>
-          <t>월11</t>
+          <t>월2,목13</t>
         </is>
       </c>
       <c r="K306" t="inlineStr">
         <is>
-          <t>다니엘관B102호(大)(자유전공학부 전용)</t>
+          <t>다니엘관B101호(大)(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L306" t="inlineStr">
@@ -18984,12 +18984,12 @@
       </c>
       <c r="J307" t="inlineStr">
         <is>
-          <t>화11</t>
+          <t>월4,목13</t>
         </is>
       </c>
       <c r="K307" t="inlineStr">
         <is>
-          <t>다니엘관B102호(大)(자유전공학부 전용)</t>
+          <t>다니엘관B102호(大)(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L307" t="inlineStr">
@@ -19048,12 +19048,12 @@
       </c>
       <c r="J308" t="inlineStr">
         <is>
-          <t>화11</t>
+          <t>월4,목13</t>
         </is>
       </c>
       <c r="K308" t="inlineStr">
         <is>
-          <t>다니엘관107호(자유전공학부 전용)</t>
+          <t>다니엘관107호(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L308" t="inlineStr">
@@ -19112,12 +19112,12 @@
       </c>
       <c r="J309" t="inlineStr">
         <is>
-          <t>수11</t>
+          <t>목13,목4</t>
         </is>
       </c>
       <c r="K309" t="inlineStr">
         <is>
-          <t>다니엘관107호(자유전공학부 전용)</t>
+          <t>다니엘관107호(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L309" t="inlineStr">
@@ -19176,12 +19176,12 @@
       </c>
       <c r="J310" t="inlineStr">
         <is>
-          <t>수11</t>
+          <t>목13,목4</t>
         </is>
       </c>
       <c r="K310" t="inlineStr">
         <is>
-          <t>다니엘관B101호(大)(자유전공학부 전용)</t>
+          <t>다니엘관B101호(大)(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L310" t="inlineStr">
@@ -19235,17 +19235,17 @@
       </c>
       <c r="I311" t="inlineStr">
         <is>
-          <t>노동욱</t>
+          <t>김향일</t>
         </is>
       </c>
       <c r="J311" t="inlineStr">
         <is>
-          <t>목11</t>
+          <t>목13,목2</t>
         </is>
       </c>
       <c r="K311" t="inlineStr">
         <is>
-          <t>다니엘관B101호(大)(자유전공학부 전용)</t>
+          <t>다니엘관B102호(大)(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L311" t="inlineStr">
@@ -19304,12 +19304,12 @@
       </c>
       <c r="J312" t="inlineStr">
         <is>
-          <t>목11</t>
+          <t>목13,목2</t>
         </is>
       </c>
       <c r="K312" t="inlineStr">
         <is>
-          <t>다니엘관107호(자유전공학부 전용)</t>
+          <t>다니엘관107호(자유전공학부 전용),온라인(가상공간)</t>
         </is>
       </c>
       <c r="L312" t="inlineStr">
@@ -19433,7 +19433,11 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I314" t="inlineStr"/>
+      <c r="I314" t="inlineStr">
+        <is>
+          <t>박건춘</t>
+        </is>
+      </c>
       <c r="J314" t="inlineStr">
         <is>
           <t>화5~6</t>
@@ -19441,7 +19445,7 @@
       </c>
       <c r="K314" t="inlineStr">
         <is>
-          <t>다니엘관107호(자유전공학부 전용)</t>
+          <t>다니엘관B101호(大)(자유전공학부 전용)</t>
         </is>
       </c>
       <c r="L314" t="inlineStr">
@@ -19497,7 +19501,11 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I315" t="inlineStr"/>
+      <c r="I315" t="inlineStr">
+        <is>
+          <t>허상민</t>
+        </is>
+      </c>
       <c r="J315" t="inlineStr">
         <is>
           <t>화7~8</t>
@@ -19505,7 +19513,7 @@
       </c>
       <c r="K315" t="inlineStr">
         <is>
-          <t>다니엘관B101호(大)(자유전공학부 전용)</t>
+          <t>다니엘관107호(자유전공학부 전용)</t>
         </is>
       </c>
       <c r="L315" t="inlineStr">
@@ -19561,7 +19569,11 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I316" t="inlineStr"/>
+      <c r="I316" t="inlineStr">
+        <is>
+          <t>강민승</t>
+        </is>
+      </c>
       <c r="J316" t="inlineStr">
         <is>
           <t>화7~8</t>
@@ -19625,7 +19637,11 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I317" t="inlineStr"/>
+      <c r="I317" t="inlineStr">
+        <is>
+          <t>박건춘</t>
+        </is>
+      </c>
       <c r="J317" t="inlineStr">
         <is>
           <t>화7~8</t>
@@ -19633,7 +19649,7 @@
       </c>
       <c r="K317" t="inlineStr">
         <is>
-          <t>다니엘관107호(자유전공학부 전용)</t>
+          <t>다니엘관B101호(大)(자유전공학부 전용)</t>
         </is>
       </c>
       <c r="L317" t="inlineStr">
@@ -19701,7 +19717,7 @@
       </c>
       <c r="K318" t="inlineStr">
         <is>
-          <t>다니엘관B101호(大)(자유전공학부 전용)</t>
+          <t>다니엘관107호(자유전공학부 전용)</t>
         </is>
       </c>
       <c r="L318" t="inlineStr">
@@ -20261,7 +20277,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I328" t="inlineStr"/>
+      <c r="I328" t="inlineStr">
+        <is>
+          <t>김연규</t>
+        </is>
+      </c>
       <c r="J328" t="inlineStr">
         <is>
           <t>수6~9,금10~11</t>
@@ -20380,7 +20400,7 @@
       </c>
       <c r="J330" t="inlineStr">
         <is>
-          <t>월5~8,금10~11</t>
+          <t>월6~9,금10~11</t>
         </is>
       </c>
       <c r="K330" t="inlineStr">
@@ -20440,7 +20460,7 @@
       </c>
       <c r="J331" t="inlineStr">
         <is>
-          <t>월5~8,금10~11</t>
+          <t>월6~9,금10~11</t>
         </is>
       </c>
       <c r="K331" t="inlineStr">
@@ -20500,7 +20520,7 @@
       </c>
       <c r="J332" t="inlineStr">
         <is>
-          <t>목5~8,금10~11</t>
+          <t>목6~9,금10~11</t>
         </is>
       </c>
       <c r="K332" t="inlineStr">
@@ -20560,7 +20580,7 @@
       </c>
       <c r="J333" t="inlineStr">
         <is>
-          <t>목5~8,금10~11</t>
+          <t>목6~9,금10~11</t>
         </is>
       </c>
       <c r="K333" t="inlineStr">
@@ -20613,7 +20633,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I334" t="inlineStr"/>
+      <c r="I334" t="inlineStr">
+        <is>
+          <t>김연규</t>
+        </is>
+      </c>
       <c r="J334" t="inlineStr">
         <is>
           <t>수1~4,금10~11</t>
@@ -25317,7 +25341,7 @@
       </c>
       <c r="K412" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>체육관308호(中)강의실</t>
         </is>
       </c>
       <c r="L412" t="inlineStr">
@@ -25773,7 +25797,7 @@
       </c>
       <c r="K420" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>체육관309호(中)강의실</t>
         </is>
       </c>
       <c r="L420" t="inlineStr">
@@ -27805,7 +27829,11 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I455" t="inlineStr"/>
+      <c r="I455" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="J455" t="inlineStr">
         <is>
           <t>화8</t>
@@ -28821,7 +28849,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I472" t="inlineStr"/>
+      <c r="I472" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="J472" t="inlineStr"/>
       <c r="K472" t="inlineStr"/>
       <c r="L472" t="inlineStr">
@@ -29289,7 +29321,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I480" t="inlineStr"/>
+      <c r="I480" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="J480" t="inlineStr"/>
       <c r="K480" t="inlineStr"/>
       <c r="L480" t="inlineStr">
@@ -29869,7 +29905,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I490" t="inlineStr"/>
+      <c r="I490" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="J490" t="inlineStr">
         <is>
           <t>금1~4</t>
@@ -30405,7 +30445,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I499" t="inlineStr"/>
+      <c r="I499" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="J499" t="inlineStr">
         <is>
           <t>금5~7</t>
@@ -30873,7 +30917,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I507" t="inlineStr"/>
+      <c r="I507" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="J507" t="inlineStr"/>
       <c r="K507" t="inlineStr"/>
       <c r="L507" t="inlineStr">
@@ -37556,12 +37604,12 @@
       </c>
       <c r="J618" t="inlineStr">
         <is>
-          <t>월5~7</t>
+          <t>월2~4</t>
         </is>
       </c>
       <c r="K618" t="inlineStr">
         <is>
-          <t>다니엘관403호(PBL)강의실</t>
+          <t>요한관422호(中)강의실</t>
         </is>
       </c>
       <c r="L618" t="inlineStr">
@@ -37676,12 +37724,12 @@
       </c>
       <c r="J620" t="inlineStr">
         <is>
-          <t>월8~10</t>
+          <t>수2~4</t>
         </is>
       </c>
       <c r="K620" t="inlineStr">
         <is>
-          <t>다니엘관403호(PBL)강의실</t>
+          <t>제2과학관407-1호(생과세미나실)</t>
         </is>
       </c>
       <c r="L620" t="inlineStr">
@@ -37736,12 +37784,12 @@
       </c>
       <c r="J621" t="inlineStr">
         <is>
-          <t>수2~4</t>
+          <t>월6~8</t>
         </is>
       </c>
       <c r="K621" t="inlineStr">
         <is>
-          <t>다니엘관405호(大)강의실</t>
+          <t>다니엘관403호(PBL)강의실</t>
         </is>
       </c>
       <c r="L621" t="inlineStr">
@@ -42077,7 +42125,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I693" t="inlineStr"/>
+      <c r="I693" t="inlineStr">
+        <is>
+          <t>김종완</t>
+        </is>
+      </c>
       <c r="J693" t="inlineStr">
         <is>
           <t>월1~3</t>
@@ -42421,7 +42473,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I699" t="inlineStr"/>
+      <c r="I699" t="inlineStr">
+        <is>
+          <t>김종완</t>
+        </is>
+      </c>
       <c r="J699" t="inlineStr">
         <is>
           <t>목12~14</t>
@@ -42717,7 +42773,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I704" t="inlineStr"/>
+      <c r="I704" t="inlineStr">
+        <is>
+          <t>김종완</t>
+        </is>
+      </c>
       <c r="J704" t="inlineStr">
         <is>
           <t>월1~3</t>
@@ -43061,7 +43121,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I710" t="inlineStr"/>
+      <c r="I710" t="inlineStr">
+        <is>
+          <t>김종완</t>
+        </is>
+      </c>
       <c r="J710" t="inlineStr">
         <is>
           <t>목12~14</t>
@@ -43357,7 +43421,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I715" t="inlineStr"/>
+      <c r="I715" t="inlineStr">
+        <is>
+          <t>김종완</t>
+        </is>
+      </c>
       <c r="J715" t="inlineStr">
         <is>
           <t>월1~3</t>
@@ -43701,7 +43769,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I721" t="inlineStr"/>
+      <c r="I721" t="inlineStr">
+        <is>
+          <t>김종완</t>
+        </is>
+      </c>
       <c r="J721" t="inlineStr">
         <is>
           <t>목12~14</t>
@@ -44536,7 +44608,7 @@
       </c>
       <c r="J735" t="inlineStr">
         <is>
-          <t>화8</t>
+          <t>월8</t>
         </is>
       </c>
       <c r="K735" t="inlineStr">
@@ -49503,7 +49575,7 @@
       </c>
       <c r="I817" t="inlineStr">
         <is>
-          <t>최성숙</t>
+          <t>강사</t>
         </is>
       </c>
       <c r="J817" t="inlineStr">
@@ -49688,7 +49760,7 @@
       </c>
       <c r="J820" t="inlineStr">
         <is>
-          <t>월1~3</t>
+          <t>월1~4</t>
         </is>
       </c>
       <c r="K820" t="inlineStr">
@@ -49928,7 +50000,7 @@
       </c>
       <c r="J824" t="inlineStr">
         <is>
-          <t>월5~7</t>
+          <t>월6~8</t>
         </is>
       </c>
       <c r="K824" t="inlineStr">
@@ -52065,11 +52137,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I858" t="inlineStr">
-        <is>
-          <t>미지정</t>
-        </is>
-      </c>
+      <c r="I858" t="inlineStr"/>
       <c r="J858" t="inlineStr">
         <is>
           <t>화4~6</t>
@@ -52901,7 +52969,11 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M871" t="inlineStr"/>
+      <c r="M871" t="inlineStr">
+        <is>
+          <t>영어 강좌</t>
+        </is>
+      </c>
       <c r="N871" t="inlineStr"/>
     </row>
     <row r="872">
@@ -53155,17 +53227,17 @@
     <row r="876">
       <c r="A876" t="inlineStr">
         <is>
-          <t>1457</t>
+          <t>1836</t>
         </is>
       </c>
       <c r="B876" t="inlineStr">
         <is>
-          <t>1001698</t>
+          <t>1007296</t>
         </is>
       </c>
       <c r="C876" t="inlineStr">
         <is>
-          <t>무역개론</t>
+          <t>무역개론(ENG)</t>
         </is>
       </c>
       <c r="D876" t="inlineStr">
@@ -53196,7 +53268,7 @@
       </c>
       <c r="J876" t="inlineStr">
         <is>
-          <t>월5~7</t>
+          <t>화5~7</t>
         </is>
       </c>
       <c r="K876" t="inlineStr">
@@ -53209,7 +53281,11 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M876" t="inlineStr"/>
+      <c r="M876" t="inlineStr">
+        <is>
+          <t>영어 강좌</t>
+        </is>
+      </c>
       <c r="N876" t="inlineStr"/>
     </row>
     <row r="877">
@@ -53329,7 +53405,11 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M878" t="inlineStr"/>
+      <c r="M878" t="inlineStr">
+        <is>
+          <t>영어 강좌</t>
+        </is>
+      </c>
       <c r="N878" t="inlineStr"/>
     </row>
     <row r="879">
@@ -54057,7 +54137,11 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M890" t="inlineStr"/>
+      <c r="M890" t="inlineStr">
+        <is>
+          <t>영어 강좌</t>
+        </is>
+      </c>
       <c r="N890" t="inlineStr"/>
     </row>
     <row r="891">
@@ -57220,7 +57304,7 @@
       </c>
       <c r="J941" t="inlineStr">
         <is>
-          <t>월6~7</t>
+          <t>금3~4</t>
         </is>
       </c>
       <c r="K941" t="inlineStr">
@@ -58637,7 +58721,7 @@
       </c>
       <c r="C963" t="inlineStr">
         <is>
-          <t>AI 웰니스 프로젝트</t>
+          <t>AI 웰니스 융합 프로젝트</t>
         </is>
       </c>
       <c r="D963" t="inlineStr">
@@ -60289,7 +60373,7 @@
       </c>
       <c r="K987" t="inlineStr">
         <is>
-          <t>다니엘관401호(PBL)강의실</t>
+          <t>신학관208호(PBL소형)강의실</t>
         </is>
       </c>
       <c r="L987" t="inlineStr">
@@ -60629,7 +60713,7 @@
       </c>
       <c r="K992" t="inlineStr">
         <is>
-          <t>사무엘관209호강의실</t>
+          <t>에스라관209호강의실(교직과목)(첨단강의실)</t>
         </is>
       </c>
       <c r="L992" t="inlineStr">
@@ -63757,7 +63841,7 @@
       </c>
       <c r="G1039" t="inlineStr">
         <is>
-          <t>자연과학영역</t>
+          <t>사회과학영역</t>
         </is>
       </c>
       <c r="H1039" t="inlineStr">
@@ -63787,7 +63871,7 @@
       </c>
       <c r="M1039" t="inlineStr">
         <is>
-          <t>자연과학영역</t>
+          <t>사회과학영역</t>
         </is>
       </c>
       <c r="N1039" t="inlineStr"/>
@@ -67048,12 +67132,12 @@
       </c>
       <c r="J1088" t="inlineStr">
         <is>
-          <t>금2~4</t>
+          <t>수1~3</t>
         </is>
       </c>
       <c r="K1088" t="inlineStr">
         <is>
-          <t>다니엘관406호(PBL 전용 Lab. 中)강의실</t>
+          <t>신학관202호강의실(PBL)</t>
         </is>
       </c>
       <c r="L1088" t="inlineStr">
@@ -67461,7 +67545,7 @@
       </c>
       <c r="K1094" t="inlineStr">
         <is>
-          <t>에스라관209호강의실(교직과목)(첨단강의실)</t>
+          <t>사무엘관209호강의실</t>
         </is>
       </c>
       <c r="L1094" t="inlineStr">
@@ -67721,7 +67805,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1098" t="inlineStr"/>
+      <c r="I1098" t="inlineStr">
+        <is>
+          <t>온라인강의교수</t>
+        </is>
+      </c>
       <c r="J1098" t="inlineStr"/>
       <c r="K1098" t="inlineStr"/>
       <c r="L1098" t="inlineStr">
@@ -67731,7 +67819,7 @@
       </c>
       <c r="M1098" t="inlineStr">
         <is>
-          <t>자연과학영역</t>
+          <t>자연과학영역, 한양대 컨소시엄 교과목</t>
         </is>
       </c>
       <c r="N1098" t="inlineStr"/>
@@ -70353,11 +70441,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1137" t="inlineStr">
-        <is>
-          <t>노현아</t>
-        </is>
-      </c>
+      <c r="I1137" t="inlineStr"/>
       <c r="J1137" t="inlineStr">
         <is>
           <t>목4~6</t>
@@ -70829,7 +70913,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1144" t="inlineStr"/>
+      <c r="I1144" t="inlineStr">
+        <is>
+          <t>온라인강의교수</t>
+        </is>
+      </c>
       <c r="J1144" t="inlineStr"/>
       <c r="K1144" t="inlineStr"/>
       <c r="L1144" t="inlineStr">
@@ -70839,7 +70927,7 @@
       </c>
       <c r="M1144" t="inlineStr">
         <is>
-          <t>디지털 리터러시영역</t>
+          <t>디지털 리터러시영역, 한양대 컨소시엄 교과목</t>
         </is>
       </c>
       <c r="N1144" t="inlineStr"/>
@@ -71361,7 +71449,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1152" t="inlineStr"/>
+      <c r="I1152" t="inlineStr">
+        <is>
+          <t>온라인강의교수</t>
+        </is>
+      </c>
       <c r="J1152" t="inlineStr"/>
       <c r="K1152" t="inlineStr"/>
       <c r="L1152" t="inlineStr">
@@ -71371,7 +71463,7 @@
       </c>
       <c r="M1152" t="inlineStr">
         <is>
-          <t>자연과학영역</t>
+          <t>자연과학영역, 한양대 컨소시엄 교과목</t>
         </is>
       </c>
       <c r="N1152" t="inlineStr"/>
@@ -72561,7 +72653,7 @@
       </c>
       <c r="K1171" t="inlineStr">
         <is>
-          <t>에스라관209호강의실(교직과목)(첨단강의실)</t>
+          <t>에스라관113호강의실</t>
         </is>
       </c>
       <c r="L1171" t="inlineStr">
@@ -72681,7 +72773,7 @@
       </c>
       <c r="K1173" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>에스라관113호강의실</t>
         </is>
       </c>
       <c r="L1173" t="inlineStr">
@@ -73117,7 +73209,7 @@
       </c>
       <c r="K1180" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>에스라관113호강의실</t>
         </is>
       </c>
       <c r="L1180" t="inlineStr">
@@ -74924,7 +75016,7 @@
       </c>
       <c r="J1210" t="inlineStr">
         <is>
-          <t>화2~4</t>
+          <t>화1~3</t>
         </is>
       </c>
       <c r="K1210" t="inlineStr">
@@ -75044,7 +75136,7 @@
       </c>
       <c r="J1212" t="inlineStr">
         <is>
-          <t>화6~8</t>
+          <t>화5~7</t>
         </is>
       </c>
       <c r="K1212" t="inlineStr">
@@ -92800,7 +92892,7 @@
       </c>
       <c r="J1503" t="inlineStr">
         <is>
-          <t>월4~5</t>
+          <t>금5~6</t>
         </is>
       </c>
       <c r="K1503" t="inlineStr">
@@ -94605,7 +94697,7 @@
       </c>
       <c r="K1533" t="inlineStr">
         <is>
-          <t>요한관 홍명기홀(강당)</t>
+          <t>다니엘관305호(大)</t>
         </is>
       </c>
       <c r="L1533" t="inlineStr">
@@ -94729,7 +94821,7 @@
       </c>
       <c r="K1535" t="inlineStr">
         <is>
-          <t>요한관 홍명기홀(강당)</t>
+          <t>다니엘관305호(大)</t>
         </is>
       </c>
       <c r="L1535" t="inlineStr">
@@ -95244,7 +95336,7 @@
       </c>
       <c r="F1544" t="inlineStr">
         <is>
-          <t>전공선택</t>
+          <t>전공필수</t>
         </is>
       </c>
       <c r="G1544" t="inlineStr"/>
@@ -95348,7 +95440,7 @@
       </c>
       <c r="F1546" t="inlineStr">
         <is>
-          <t>전공선택</t>
+          <t>전공필수</t>
         </is>
       </c>
       <c r="G1546" t="inlineStr"/>
@@ -95408,7 +95500,7 @@
       </c>
       <c r="F1547" t="inlineStr">
         <is>
-          <t>전공선택</t>
+          <t>전공필수</t>
         </is>
       </c>
       <c r="G1547" t="inlineStr"/>

</xml_diff>

<commit_message>
chore(data): add 2026-1 data files ('26.01.26)
</commit_message>
<xml_diff>
--- a/data/2026년 1학기 정규 시간표.xlsx
+++ b/data/2026년 1학기 정규 시간표.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1599"/>
+  <dimension ref="A1:N1602"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5990,7 +5990,11 @@
         </is>
       </c>
       <c r="M92" t="inlineStr"/>
-      <c r="N92" t="inlineStr"/>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>(팀티칭)</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -6050,7 +6054,11 @@
         </is>
       </c>
       <c r="M93" t="inlineStr"/>
-      <c r="N93" t="inlineStr"/>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>(팀티칭)</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -12373,7 +12381,7 @@
       </c>
       <c r="K198" t="inlineStr">
         <is>
-          <t>디자인관209호(건축학과Studio)</t>
+          <t>디자인관210호(건축학과Studio)</t>
         </is>
       </c>
       <c r="L198" t="inlineStr">
@@ -13266,8 +13274,16 @@
         </is>
       </c>
       <c r="I213" t="inlineStr"/>
-      <c r="J213" t="inlineStr"/>
-      <c r="K213" t="inlineStr"/>
+      <c r="J213" t="inlineStr">
+        <is>
+          <t>목1~3</t>
+        </is>
+      </c>
+      <c r="K213" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L213" t="inlineStr">
         <is>
           <t>미래융합대학</t>
@@ -22856,7 +22872,7 @@
       <c r="I369" t="inlineStr"/>
       <c r="J369" t="inlineStr">
         <is>
-          <t>화6~8</t>
+          <t>화5~7</t>
         </is>
       </c>
       <c r="K369" t="inlineStr">
@@ -40424,7 +40440,7 @@
       </c>
       <c r="J660" t="inlineStr">
         <is>
-          <t>화5~7</t>
+          <t>금5~7</t>
         </is>
       </c>
       <c r="K660" t="inlineStr">
@@ -54549,11 +54565,7 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M891" t="inlineStr">
-        <is>
-          <t>영어 강좌</t>
-        </is>
-      </c>
+      <c r="M891" t="inlineStr"/>
       <c r="N891" t="inlineStr"/>
     </row>
     <row r="892">
@@ -59071,7 +59083,7 @@
       </c>
       <c r="M963" t="inlineStr">
         <is>
-          <t>일반선택영역</t>
+          <t>일반선택영역, 항공관광외국어학부 신청불가</t>
         </is>
       </c>
       <c r="N963" t="inlineStr"/>
@@ -59971,7 +59983,7 @@
       </c>
       <c r="M977" t="inlineStr">
         <is>
-          <t>일반선택영역</t>
+          <t>일반선택영역, 체육학과 신청불가</t>
         </is>
       </c>
       <c r="N977" t="inlineStr"/>
@@ -61195,7 +61207,7 @@
       </c>
       <c r="M995" t="inlineStr">
         <is>
-          <t>자연과학영역, 생활체육학과 신청불가</t>
+          <t>자연과학영역, 체육학과 신청불가</t>
         </is>
       </c>
       <c r="N995" t="inlineStr"/>
@@ -65995,7 +66007,7 @@
       </c>
       <c r="M1066" t="inlineStr">
         <is>
-          <t>일반선택영역</t>
+          <t>일반선택영역, 외국인학생만 신청가능</t>
         </is>
       </c>
       <c r="N1066" t="inlineStr"/>
@@ -66255,7 +66267,7 @@
       </c>
       <c r="M1070" t="inlineStr">
         <is>
-          <t>일반선택영역</t>
+          <t>일반선택영역, 외국인학생만 신청가능</t>
         </is>
       </c>
       <c r="N1070" t="inlineStr"/>
@@ -82227,7 +82239,7 @@
       </c>
       <c r="I1322" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>김태중</t>
         </is>
       </c>
       <c r="J1322" t="inlineStr">
@@ -82287,7 +82299,7 @@
       </c>
       <c r="I1323" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>김태중</t>
         </is>
       </c>
       <c r="J1323" t="inlineStr">
@@ -85835,7 +85847,7 @@
       </c>
       <c r="M1381" t="inlineStr">
         <is>
-          <t>핵심교양</t>
+          <t>핵심교양, 유아교육과 학생만 수강 가능합니다.</t>
         </is>
       </c>
       <c r="N1381" t="inlineStr"/>
@@ -86391,7 +86403,7 @@
       </c>
       <c r="M1390" t="inlineStr">
         <is>
-          <t>핵심교양</t>
+          <t>핵심교양, 유아교육과 학생만 수강 가능합니다.</t>
         </is>
       </c>
       <c r="N1390" t="inlineStr"/>
@@ -98887,17 +98899,17 @@
     <row r="1594">
       <c r="A1594" t="inlineStr">
         <is>
-          <t>1608</t>
+          <t>1595</t>
         </is>
       </c>
       <c r="B1594" t="inlineStr">
         <is>
-          <t>1006564</t>
+          <t>1004601</t>
         </is>
       </c>
       <c r="C1594" t="inlineStr">
         <is>
-          <t>채플(온라인)</t>
+          <t>졸업연구</t>
         </is>
       </c>
       <c r="D1594" t="inlineStr">
@@ -98912,7 +98924,7 @@
       </c>
       <c r="F1594" t="inlineStr">
         <is>
-          <t>채플</t>
+          <t>전공필수</t>
         </is>
       </c>
       <c r="G1594" t="inlineStr"/>
@@ -98923,17 +98935,17 @@
       </c>
       <c r="I1594" t="inlineStr">
         <is>
-          <t>김영수</t>
+          <t>유예진</t>
         </is>
       </c>
       <c r="J1594" t="inlineStr">
         <is>
-          <t>금12</t>
+          <t>목12</t>
         </is>
       </c>
       <c r="K1594" t="inlineStr">
         <is>
-          <t>온라인(가상공간)</t>
+          <t>바울관413호식음료실습실</t>
         </is>
       </c>
       <c r="L1594" t="inlineStr">
@@ -98951,17 +98963,17 @@
     <row r="1595">
       <c r="A1595" t="inlineStr">
         <is>
-          <t>1593</t>
+          <t>1595</t>
         </is>
       </c>
       <c r="B1595" t="inlineStr">
         <is>
-          <t>1000693</t>
+          <t>1004601</t>
         </is>
       </c>
       <c r="C1595" t="inlineStr">
         <is>
-          <t>고급중국어</t>
+          <t>졸업연구</t>
         </is>
       </c>
       <c r="D1595" t="inlineStr">
@@ -98976,28 +98988,28 @@
       </c>
       <c r="F1595" t="inlineStr">
         <is>
-          <t>전공선택</t>
+          <t>전공필수</t>
         </is>
       </c>
       <c r="G1595" t="inlineStr"/>
       <c r="H1595" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I1595" t="inlineStr">
         <is>
-          <t>안병삼</t>
+          <t>유예진</t>
         </is>
       </c>
       <c r="J1595" t="inlineStr">
         <is>
-          <t>목2~4</t>
+          <t>목12</t>
         </is>
       </c>
       <c r="K1595" t="inlineStr">
         <is>
-          <t>다니엘관301호(中)강의실</t>
+          <t>바울관413호식음료실습실</t>
         </is>
       </c>
       <c r="L1595" t="inlineStr">
@@ -99006,22 +99018,26 @@
         </is>
       </c>
       <c r="M1595" t="inlineStr"/>
-      <c r="N1595" t="inlineStr"/>
+      <c r="N1595" t="inlineStr">
+        <is>
+          <t>(팀티칭)</t>
+        </is>
+      </c>
     </row>
     <row r="1596">
       <c r="A1596" t="inlineStr">
         <is>
-          <t>1613</t>
+          <t>1595</t>
         </is>
       </c>
       <c r="B1596" t="inlineStr">
         <is>
-          <t>1007002</t>
+          <t>1004601</t>
         </is>
       </c>
       <c r="C1596" t="inlineStr">
         <is>
-          <t>관광서비스혁신</t>
+          <t>졸업연구</t>
         </is>
       </c>
       <c r="D1596" t="inlineStr">
@@ -99036,28 +99052,28 @@
       </c>
       <c r="F1596" t="inlineStr">
         <is>
-          <t>전공선택</t>
+          <t>전공필수</t>
         </is>
       </c>
       <c r="G1596" t="inlineStr"/>
       <c r="H1596" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I1596" t="inlineStr">
         <is>
-          <t>민세원</t>
+          <t>유예진</t>
         </is>
       </c>
       <c r="J1596" t="inlineStr">
         <is>
-          <t>금6~8</t>
+          <t>목12</t>
         </is>
       </c>
       <c r="K1596" t="inlineStr">
         <is>
-          <t>바울관403호강의실</t>
+          <t>바울관413호식음료실습실</t>
         </is>
       </c>
       <c r="L1596" t="inlineStr">
@@ -99066,22 +99082,26 @@
         </is>
       </c>
       <c r="M1596" t="inlineStr"/>
-      <c r="N1596" t="inlineStr"/>
+      <c r="N1596" t="inlineStr">
+        <is>
+          <t>(팀티칭)</t>
+        </is>
+      </c>
     </row>
     <row r="1597">
       <c r="A1597" t="inlineStr">
         <is>
-          <t>1631</t>
+          <t>1608</t>
         </is>
       </c>
       <c r="B1597" t="inlineStr">
         <is>
-          <t>1006847</t>
+          <t>1006564</t>
         </is>
       </c>
       <c r="C1597" t="inlineStr">
         <is>
-          <t>서비스 롤플레이</t>
+          <t>채플(온라인)</t>
         </is>
       </c>
       <c r="D1597" t="inlineStr">
@@ -99096,24 +99116,28 @@
       </c>
       <c r="F1597" t="inlineStr">
         <is>
-          <t>전공선택</t>
+          <t>채플</t>
         </is>
       </c>
       <c r="G1597" t="inlineStr"/>
       <c r="H1597" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I1597" t="inlineStr"/>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I1597" t="inlineStr">
+        <is>
+          <t>김영수</t>
+        </is>
+      </c>
       <c r="J1597" t="inlineStr">
         <is>
-          <t>화2~4</t>
+          <t>금12</t>
         </is>
       </c>
       <c r="K1597" t="inlineStr">
         <is>
-          <t>바울관401호항공실습실</t>
+          <t>온라인(가상공간)</t>
         </is>
       </c>
       <c r="L1597" t="inlineStr">
@@ -99122,22 +99146,26 @@
         </is>
       </c>
       <c r="M1597" t="inlineStr"/>
-      <c r="N1597" t="inlineStr"/>
+      <c r="N1597" t="inlineStr">
+        <is>
+          <t>(팀티칭)</t>
+        </is>
+      </c>
     </row>
     <row r="1598">
       <c r="A1598" t="inlineStr">
         <is>
-          <t>1618</t>
+          <t>1593</t>
         </is>
       </c>
       <c r="B1598" t="inlineStr">
         <is>
-          <t>1007006</t>
+          <t>1000693</t>
         </is>
       </c>
       <c r="C1598" t="inlineStr">
         <is>
-          <t>융합캡스톤디자인(일본어)</t>
+          <t>고급중국어</t>
         </is>
       </c>
       <c r="D1598" t="inlineStr">
@@ -99163,17 +99191,17 @@
       </c>
       <c r="I1598" t="inlineStr">
         <is>
-          <t>유예진</t>
+          <t>안병삼</t>
         </is>
       </c>
       <c r="J1598" t="inlineStr">
         <is>
-          <t>화6~8</t>
+          <t>목2~4</t>
         </is>
       </c>
       <c r="K1598" t="inlineStr">
         <is>
-          <t>바울관413호식음료실습실</t>
+          <t>다니엘관301호(中)강의실</t>
         </is>
       </c>
       <c r="L1598" t="inlineStr">
@@ -99187,17 +99215,17 @@
     <row r="1599">
       <c r="A1599" t="inlineStr">
         <is>
-          <t>1627</t>
+          <t>1613</t>
         </is>
       </c>
       <c r="B1599" t="inlineStr">
         <is>
-          <t>1005215</t>
+          <t>1007002</t>
         </is>
       </c>
       <c r="C1599" t="inlineStr">
         <is>
-          <t>한중번역 및 통역</t>
+          <t>관광서비스혁신</t>
         </is>
       </c>
       <c r="D1599" t="inlineStr">
@@ -99223,12 +99251,12 @@
       </c>
       <c r="I1599" t="inlineStr">
         <is>
-          <t>박민수</t>
+          <t>민세원</t>
         </is>
       </c>
       <c r="J1599" t="inlineStr">
         <is>
-          <t>목6~8</t>
+          <t>금6~8</t>
         </is>
       </c>
       <c r="K1599" t="inlineStr">
@@ -99243,6 +99271,182 @@
       </c>
       <c r="M1599" t="inlineStr"/>
       <c r="N1599" t="inlineStr"/>
+    </row>
+    <row r="1600">
+      <c r="A1600" t="inlineStr">
+        <is>
+          <t>1631</t>
+        </is>
+      </c>
+      <c r="B1600" t="inlineStr">
+        <is>
+          <t>1006847</t>
+        </is>
+      </c>
+      <c r="C1600" t="inlineStr">
+        <is>
+          <t>서비스 롤플레이</t>
+        </is>
+      </c>
+      <c r="D1600" t="inlineStr">
+        <is>
+          <t>항공관광외국어학부</t>
+        </is>
+      </c>
+      <c r="E1600" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F1600" t="inlineStr">
+        <is>
+          <t>전공선택</t>
+        </is>
+      </c>
+      <c r="G1600" t="inlineStr"/>
+      <c r="H1600" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I1600" t="inlineStr"/>
+      <c r="J1600" t="inlineStr">
+        <is>
+          <t>화2~4</t>
+        </is>
+      </c>
+      <c r="K1600" t="inlineStr">
+        <is>
+          <t>바울관401호항공실습실</t>
+        </is>
+      </c>
+      <c r="L1600" t="inlineStr">
+        <is>
+          <t>창의융합대학</t>
+        </is>
+      </c>
+      <c r="M1600" t="inlineStr"/>
+      <c r="N1600" t="inlineStr"/>
+    </row>
+    <row r="1601">
+      <c r="A1601" t="inlineStr">
+        <is>
+          <t>1618</t>
+        </is>
+      </c>
+      <c r="B1601" t="inlineStr">
+        <is>
+          <t>1007006</t>
+        </is>
+      </c>
+      <c r="C1601" t="inlineStr">
+        <is>
+          <t>융합캡스톤디자인(일본어)</t>
+        </is>
+      </c>
+      <c r="D1601" t="inlineStr">
+        <is>
+          <t>항공관광외국어학부</t>
+        </is>
+      </c>
+      <c r="E1601" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F1601" t="inlineStr">
+        <is>
+          <t>전공선택</t>
+        </is>
+      </c>
+      <c r="G1601" t="inlineStr"/>
+      <c r="H1601" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I1601" t="inlineStr">
+        <is>
+          <t>유예진</t>
+        </is>
+      </c>
+      <c r="J1601" t="inlineStr">
+        <is>
+          <t>화6~8</t>
+        </is>
+      </c>
+      <c r="K1601" t="inlineStr">
+        <is>
+          <t>바울관413호식음료실습실</t>
+        </is>
+      </c>
+      <c r="L1601" t="inlineStr">
+        <is>
+          <t>창의융합대학</t>
+        </is>
+      </c>
+      <c r="M1601" t="inlineStr"/>
+      <c r="N1601" t="inlineStr"/>
+    </row>
+    <row r="1602">
+      <c r="A1602" t="inlineStr">
+        <is>
+          <t>1627</t>
+        </is>
+      </c>
+      <c r="B1602" t="inlineStr">
+        <is>
+          <t>1005215</t>
+        </is>
+      </c>
+      <c r="C1602" t="inlineStr">
+        <is>
+          <t>한중번역 및 통역</t>
+        </is>
+      </c>
+      <c r="D1602" t="inlineStr">
+        <is>
+          <t>항공관광외국어학부</t>
+        </is>
+      </c>
+      <c r="E1602" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F1602" t="inlineStr">
+        <is>
+          <t>전공선택</t>
+        </is>
+      </c>
+      <c r="G1602" t="inlineStr"/>
+      <c r="H1602" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I1602" t="inlineStr">
+        <is>
+          <t>박민수</t>
+        </is>
+      </c>
+      <c r="J1602" t="inlineStr">
+        <is>
+          <t>목6~8</t>
+        </is>
+      </c>
+      <c r="K1602" t="inlineStr">
+        <is>
+          <t>바울관403호강의실</t>
+        </is>
+      </c>
+      <c r="L1602" t="inlineStr">
+        <is>
+          <t>창의융합대학</t>
+        </is>
+      </c>
+      <c r="M1602" t="inlineStr"/>
+      <c r="N1602" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
chore(data): add 2026-1 data files ('26.01.28)
</commit_message>
<xml_diff>
--- a/data/2026년 1학기 정규 시간표.xlsx
+++ b/data/2026년 1학기 정규 시간표.xlsx
@@ -1077,7 +1077,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>요한관422호(中)강의실</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>요한관421호(中)강의실</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>제3과학관209호(문제중심학습)</t>
+          <t>요한관323호(中)강의실</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>제3과학관221호(외래강사실)</t>
+          <t>요한관322호(中)강의실</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -34443,7 +34443,7 @@
     <row r="558">
       <c r="A558" t="inlineStr">
         <is>
-          <t>1763</t>
+          <t>1840</t>
         </is>
       </c>
       <c r="B558" t="inlineStr">
@@ -34507,7 +34507,7 @@
     <row r="559">
       <c r="A559" t="inlineStr">
         <is>
-          <t>1764</t>
+          <t>1841</t>
         </is>
       </c>
       <c r="B559" t="inlineStr">
@@ -41200,12 +41200,12 @@
       </c>
       <c r="J669" t="inlineStr">
         <is>
-          <t>목1~3</t>
+          <t>화5~7</t>
         </is>
       </c>
       <c r="K669" t="inlineStr">
         <is>
-          <t>제2과학관501-1호강의실</t>
+          <t>다니엘관204호(小)</t>
         </is>
       </c>
       <c r="L669" t="inlineStr">
@@ -43080,7 +43080,7 @@
       </c>
       <c r="J700" t="inlineStr">
         <is>
-          <t>목1~3</t>
+          <t>목2~4</t>
         </is>
       </c>
       <c r="K700" t="inlineStr">
@@ -57887,7 +57887,7 @@
       </c>
       <c r="M942" t="inlineStr">
         <is>
-          <t>교직필수, 해외교육봉사</t>
+          <t>교직필수</t>
         </is>
       </c>
       <c r="N942" t="inlineStr"/>
@@ -78373,7 +78373,11 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M1254" t="inlineStr"/>
+      <c r="M1254" t="inlineStr">
+        <is>
+          <t>상담심리학과 1학년 학생만 수강 가능(타학과, 타학년 수강 불가)</t>
+        </is>
+      </c>
       <c r="N1254" t="inlineStr"/>
     </row>
     <row r="1255">
@@ -78793,7 +78797,11 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M1261" t="inlineStr"/>
+      <c r="M1261" t="inlineStr">
+        <is>
+          <t>상담심리학과 2학년 학생만 수강 가능(타학과, 타학년 수강 불가)</t>
+        </is>
+      </c>
       <c r="N1261" t="inlineStr"/>
     </row>
     <row r="1262">
@@ -88475,7 +88483,7 @@
       </c>
       <c r="I1420" t="inlineStr">
         <is>
-          <t>오혜전</t>
+          <t>조대명</t>
         </is>
       </c>
       <c r="J1420" t="inlineStr">

</xml_diff>